<commit_message>
added update to QC pipeline
</commit_message>
<xml_diff>
--- a/16S_Clust_Gen_Pipeline/16S_Pipeline_Validation_Checklist.xlsx
+++ b/16S_Clust_Gen_Pipeline/16S_Pipeline_Validation_Checklist.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
   <si>
     <t>16S QC and Pipeline Run Validation Checklist</t>
   </si>
@@ -148,8 +148,29 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>8.)</t>
+    <t>Confirm Merge:</t>
+  </si>
+  <si>
+    <t>Confirm Mothur Run:</t>
+  </si>
+  <si>
+    <t>n=</t>
+  </si>
+  <si>
+    <t>Date:</t>
+  </si>
+  <si>
+    <t>Project Directory Name:</t>
+  </si>
+  <si>
+    <t>Done?</t>
+  </si>
+  <si>
+    <t>Validated by:</t>
+  </si>
+  <si>
+    <r>
+      <t>7.)</t>
     </r>
     <r>
       <rPr>
@@ -168,12 +189,27 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Spot check some fastq_qc_log’s</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>a.</t>
+      <t>Are there fastq_qc_log’s and timing_log’s?  (How many depends on how many nodes/parallelization)</t>
+    </r>
+  </si>
+  <si>
+    <t>(initials)</t>
+  </si>
+  <si>
+    <t>Additional Comments:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Num Control = </t>
+  </si>
+  <si>
+    <t>Num of Total =</t>
+  </si>
+  <si>
+    <t>Num Experimental =</t>
+  </si>
+  <si>
+    <r>
+      <t>5.)</t>
     </r>
     <r>
       <rPr>
@@ -182,7 +218,7 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve">       </t>
+      <t xml:space="preserve">    </t>
     </r>
     <r>
       <rPr>
@@ -192,12 +228,15 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Do you see entries for both Forward, Reverse for the steps specified in run?</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>b.</t>
+      <t>How many samples are there?  (count number of R1 and R2 files to confirm everything is paired)</t>
+    </r>
+  </si>
+  <si>
+    <t>(Version: Feb 21, 2020)</t>
+  </si>
+  <si>
+    <r>
+      <t>8.)</t>
     </r>
     <r>
       <rPr>
@@ -206,7 +245,7 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve">      </t>
+      <t xml:space="preserve">   </t>
     </r>
     <r>
       <rPr>
@@ -216,36 +255,18 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Do you see a final paired/merged entry?</t>
-    </r>
-  </si>
-  <si>
-    <t>Confirm Merge:</t>
-  </si>
-  <si>
-    <t>Confirm Mothur Run:</t>
-  </si>
-  <si>
-    <t>(Version: Feb 17, 2020)</t>
-  </si>
-  <si>
-    <t>n=</t>
-  </si>
-  <si>
-    <t>Date:</t>
-  </si>
-  <si>
-    <t>Project Directory Name:</t>
-  </si>
-  <si>
-    <t>Done?</t>
-  </si>
-  <si>
-    <t>Validated by:</t>
-  </si>
-  <si>
-    <r>
-      <t>7.)</t>
+      <t>Run the Run_QC_PostProc.r script</t>
+    </r>
+  </si>
+  <si>
+    <t>10.) Did the number of log files read in match the level of parallelization the pipeline was run?</t>
+  </si>
+  <si>
+    <t>11.) How many total samples were there?</t>
+  </si>
+  <si>
+    <r>
+      <t>13.)</t>
     </r>
     <r>
       <rPr>
@@ -254,7 +275,7 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve">    </t>
+      <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
@@ -264,27 +285,12 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Are there fastq_qc_log’s and timing_log’s?  (How many depends on how many nodes/parallelization)</t>
-    </r>
-  </si>
-  <si>
-    <t>9.)  Perform: grep -G "paired\smerged" fastq_qc_log.*.tsv &gt; merged.fastq_log.tsv</t>
-  </si>
-  <si>
-    <t>10.) Perform: wc -l merged.fastq_log.tsv, how many samples are there?</t>
-  </si>
-  <si>
-    <t>(initials)</t>
-  </si>
-  <si>
-    <t>Additional Comments:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Num Control = </t>
-  </si>
-  <si>
-    <r>
-      <t>13.)</t>
+      <t xml:space="preserve"> In the Sequences/QV_*/MergeMates/screened_fasta directory, do you see a single file for each sample?  How many are there?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>14.)</t>
     </r>
     <r>
       <rPr>
@@ -308,7 +314,7 @@
   </si>
   <si>
     <r>
-      <t>14.)</t>
+      <t>15.)</t>
     </r>
     <r>
       <rPr>
@@ -332,7 +338,7 @@
   </si>
   <si>
     <r>
-      <t>15.)</t>
+      <t>16.)</t>
     </r>
     <r>
       <rPr>
@@ -355,14 +361,8 @@
     </r>
   </si>
   <si>
-    <t>Num of Total =</t>
-  </si>
-  <si>
-    <t>Num Experimental =</t>
-  </si>
-  <si>
-    <r>
-      <t>5.)</t>
+    <r>
+      <t>17.)</t>
     </r>
     <r>
       <rPr>
@@ -371,7 +371,7 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve">    </t>
+      <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
@@ -381,12 +381,12 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>How many samples are there?  (count number of R1 and R2 files to confirm everything is paired)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>12.)</t>
+      <t xml:space="preserve"> In the Summary_Tables directory, do you see the 6 taxonomic levels from Kingdom to Genus, and the otu.97.genus.summary_table.tsv?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>18.)</t>
     </r>
     <r>
       <rPr>
@@ -405,152 +405,88 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> In the Sequences/QV_*/MergeMates/screened_fasta directory, do you see a single file for each sample?  How many are there?</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>16.)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
+      <t xml:space="preserve"> Do you see the 8 post-mothur steps, from 01_shared_to_summary_table.log to 08_filter_samples_by_read_depth.log?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>19.) How total samples were there without filtering? See</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> In the Summary_Tables directory, do you see the 6 taxonomic levels from Kingdom to Genus, and the otu.97.genus.summary_table.tsv?</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>17.)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
+      <t xml:space="preserve"> &lt;prj_name&gt;.taxa.genus.summary.txt</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">20.) How many experimental samples are there after liberal depth filtering? See </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> Do you see the 8 post-mothur steps, from 01_shared_to_summary_table.log to 08_filter_samples_by_read_depth.log?</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">21.) Do you see the 3 .pdf files in the Descriptive directory?  </t>
-    </r>
-    <r>
-      <rPr>
+      <t>&lt;prj_name&gt;.taxa.genus.cmF.cln.exp.min_0750.summary.txt</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>21.) How many control samples were there before any filtering? See</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
         <sz val="11"/>
-        <color theme="5"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>E-mail the 3 pdf files</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>11.)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
+      <t xml:space="preserve"> &lt;prj_name&gt;.taxa.genus.cmF.cln.ctl.summary.txt</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">22.) Do you see the 3 .pdf files in the Descriptive directory?  </t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> </t>
+      <t>E-mail the 3 pdf files</t>
+    </r>
+  </si>
+  <si>
+    <t>9.)  Download and examine the summary.pdf file</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">12.) </t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="5"/>
+        <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>E-mail merged.fastq_log.tsv file.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>18.) How total samples were there without filtering? See</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> &lt;prj_name&gt;.taxa.genus.summary.txt</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>20.) How many control samples were there before any filtering? See</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> &lt;prj_name&gt;.taxa.genus.cmF.cln.ctl.summary.txt</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">19.) How many experimental samples are there after liberal depth filtering? See </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;prj_name&gt;.taxa.genus.cmF.cln.exp.min_0750.summary.txt</t>
+      <t>E-mail the QC.tgz file.</t>
     </r>
   </si>
 </sst>
@@ -605,7 +541,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="5"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -655,7 +591,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -665,9 +601,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="10"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -711,7 +644,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp10.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$B$28" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$B$30" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp11.xml><?xml version="1.0" encoding="utf-8"?>
@@ -727,11 +660,15 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp14.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$B$34" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$B$37" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp15.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$B$38" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$B$21" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp16.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$B$23" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -759,11 +696,11 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp8.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$B$22" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$B$20" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp9.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$B$24" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$B$27" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -779,7 +716,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>28575</xdr:colOff>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>8</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
@@ -843,7 +780,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>28575</xdr:colOff>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>11</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
@@ -907,7 +844,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>28575</xdr:colOff>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>12</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
@@ -971,7 +908,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>28575</xdr:colOff>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>13</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
@@ -1035,7 +972,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>28575</xdr:colOff>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>17</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
@@ -1099,7 +1036,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>28575</xdr:colOff>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>18</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
@@ -1163,7 +1100,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>28575</xdr:colOff>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>19</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
@@ -1222,14 +1159,14 @@
         <xdr:from>
           <xdr:col>3</xdr:col>
           <xdr:colOff>76200</xdr:colOff>
-          <xdr:row>20</xdr:row>
-          <xdr:rowOff>180975</xdr:rowOff>
+          <xdr:row>19</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>28575</xdr:colOff>
-          <xdr:row>22</xdr:row>
-          <xdr:rowOff>19050</xdr:rowOff>
+          <xdr:colOff>104775</xdr:colOff>
+          <xdr:row>20</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1286,77 +1223,13 @@
         <xdr:from>
           <xdr:col>3</xdr:col>
           <xdr:colOff>76200</xdr:colOff>
-          <xdr:row>22</xdr:row>
+          <xdr:row>25</xdr:row>
           <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>28575</xdr:colOff>
-          <xdr:row>24</xdr:row>
-          <xdr:rowOff>19050</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="2058" name="Check Box 10" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s2058"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>3</xdr:col>
-          <xdr:colOff>76200</xdr:colOff>
-          <xdr:row>26</xdr:row>
-          <xdr:rowOff>180975</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>4</xdr:col>
-          <xdr:colOff>28575</xdr:colOff>
-          <xdr:row>28</xdr:row>
+          <xdr:colOff>104775</xdr:colOff>
+          <xdr:row>27</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -1414,13 +1287,13 @@
         <xdr:from>
           <xdr:col>3</xdr:col>
           <xdr:colOff>76200</xdr:colOff>
-          <xdr:row>29</xdr:row>
+          <xdr:row>28</xdr:row>
           <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>28575</xdr:colOff>
-          <xdr:row>31</xdr:row>
+          <xdr:colOff>104775</xdr:colOff>
+          <xdr:row>30</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -1478,13 +1351,13 @@
         <xdr:from>
           <xdr:col>3</xdr:col>
           <xdr:colOff>76200</xdr:colOff>
-          <xdr:row>30</xdr:row>
+          <xdr:row>29</xdr:row>
           <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>28575</xdr:colOff>
-          <xdr:row>32</xdr:row>
+          <xdr:colOff>104775</xdr:colOff>
+          <xdr:row>31</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -1542,13 +1415,13 @@
         <xdr:from>
           <xdr:col>3</xdr:col>
           <xdr:colOff>76200</xdr:colOff>
-          <xdr:row>31</xdr:row>
+          <xdr:row>30</xdr:row>
           <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>28575</xdr:colOff>
-          <xdr:row>33</xdr:row>
+          <xdr:colOff>104775</xdr:colOff>
+          <xdr:row>32</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -1606,13 +1479,13 @@
         <xdr:from>
           <xdr:col>3</xdr:col>
           <xdr:colOff>76200</xdr:colOff>
-          <xdr:row>32</xdr:row>
+          <xdr:row>31</xdr:row>
           <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>28575</xdr:colOff>
-          <xdr:row>34</xdr:row>
+          <xdr:colOff>104775</xdr:colOff>
+          <xdr:row>33</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -1670,13 +1543,13 @@
         <xdr:from>
           <xdr:col>3</xdr:col>
           <xdr:colOff>76200</xdr:colOff>
-          <xdr:row>36</xdr:row>
+          <xdr:row>35</xdr:row>
           <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>28575</xdr:colOff>
-          <xdr:row>38</xdr:row>
+          <xdr:colOff>104775</xdr:colOff>
+          <xdr:row>37</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -1685,6 +1558,134 @@
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s2067"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>76200</xdr:colOff>
+          <xdr:row>19</xdr:row>
+          <xdr:rowOff>171450</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
+          <xdr:row>21</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2068" name="Check Box 20" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2068"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>76200</xdr:colOff>
+          <xdr:row>21</xdr:row>
+          <xdr:rowOff>180975</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
+          <xdr:row>23</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2069" name="Check Box 21" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2069"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2018,18 +2019,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E43"/>
+  <dimension ref="B2:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.28515625" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="13"/>
+    <col min="2" max="2" width="9.140625" style="12"/>
     <col min="3" max="3" width="8.140625" customWidth="1"/>
-    <col min="4" max="4" width="7" customWidth="1"/>
+    <col min="4" max="4" width="5.85546875" customWidth="1"/>
     <col min="5" max="5" width="102" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2040,32 +2041,32 @@
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E3" s="1" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D5" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="12"/>
+      <c r="D5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="11"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D7" s="8" t="str">
+      <c r="D7" s="7" t="str">
         <f>IF(B8, "OK", "")</f>
         <v/>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="10" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="13" t="b">
+      <c r="B8" s="12" t="b">
         <v>0</v>
       </c>
       <c r="E8" s="3" t="s">
@@ -2076,16 +2077,16 @@
       <c r="E9" s="3"/>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D10" s="8" t="str">
+      <c r="D10" s="7" t="str">
         <f>IF(AND(B11:B13), "OK", "")</f>
         <v/>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="10" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="13" t="b">
+      <c r="B11" s="12" t="b">
         <v>0</v>
       </c>
       <c r="E11" s="3" t="s">
@@ -2093,7 +2094,7 @@
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="13" t="b">
+      <c r="B12" s="12" t="b">
         <v>0</v>
       </c>
       <c r="E12" s="3" t="s">
@@ -2101,7 +2102,7 @@
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="13" t="b">
+      <c r="B13" s="12" t="b">
         <v>0</v>
       </c>
       <c r="E13" s="3" t="s">
@@ -2109,30 +2110,30 @@
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C14" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="5"/>
+      <c r="C14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="4"/>
       <c r="E14" s="3" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C15" s="6"/>
-      <c r="D15" s="7"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="6"/>
       <c r="E15" s="3"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D16" s="8" t="str">
-        <f>IF(AND(B17:B19,B22:B24), "OK", "")</f>
+      <c r="D16" s="7" t="str">
+        <f>IF(AND(B17:B19,B20:B23), "OK", "")</f>
         <v/>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="E16" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="13" t="b">
+      <c r="B17" s="12" t="b">
         <v>0</v>
       </c>
       <c r="E17" s="3" t="s">
@@ -2140,192 +2141,193 @@
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="13" t="b">
+      <c r="B18" s="12" t="b">
         <v>0</v>
       </c>
       <c r="E18" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="C20" s="13"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="C21" s="13"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C22" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="4"/>
+      <c r="E22" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E24" s="3"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D25" s="7" t="str">
+        <f>IF(AND(B26:B27),"OK","")</f>
+        <v/>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C26" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" s="4"/>
+      <c r="E26" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E28" s="3"/>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D29" s="7" t="str">
+        <f>IF(AND(B30:B37),"OK","")</f>
+        <v/>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C34" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="13" t="b">
+      <c r="D34" s="4"/>
+      <c r="E34" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C35" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D35" s="4"/>
+      <c r="E35" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C36" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D36" s="4"/>
+      <c r="E36" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B37" s="12" t="b">
         <v>0</v>
       </c>
-      <c r="E19" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E20" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D21" s="8"/>
-      <c r="E21" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C23" s="14" t="s">
+      <c r="C37" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D37" s="6"/>
+      <c r="E37" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C39" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D23" s="5"/>
-      <c r="E23" s="10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="C24" s="6" t="s">
+      <c r="D39" s="8"/>
+      <c r="E39" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C40" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D40" s="8"/>
+    </row>
+    <row r="42" spans="2:5" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D42" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E24" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E25" s="3"/>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D26" s="8" t="str">
-        <f>IF(AND(B27:B28),"OK","")</f>
-        <v/>
-      </c>
-      <c r="E26" s="11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C27" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="D27" s="5"/>
-      <c r="E27" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E29" s="3"/>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D30" s="8" t="str">
-        <f>IF(AND(B31:B38),"OK","")</f>
-        <v/>
-      </c>
-      <c r="E30" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B31" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B34" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C35" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D35" s="5"/>
-      <c r="E35" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C36" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D36" s="5"/>
-      <c r="E36" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C37" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D37" s="5"/>
-      <c r="E37" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B38" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D38" s="7"/>
-      <c r="E38" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="40" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C40" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D40" s="9"/>
-      <c r="E40" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="41" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C41" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D41" s="9"/>
-    </row>
-    <row r="43" spans="2:5" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D43" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E43" s="5"/>
+      <c r="E42" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2348,7 +2350,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>28575</xdr:colOff>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>8</xdr:row>
                     <xdr:rowOff>19050</xdr:rowOff>
                   </to>
@@ -2370,7 +2372,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>28575</xdr:colOff>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>11</xdr:row>
                     <xdr:rowOff>19050</xdr:rowOff>
                   </to>
@@ -2392,7 +2394,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>28575</xdr:colOff>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>12</xdr:row>
                     <xdr:rowOff>19050</xdr:rowOff>
                   </to>
@@ -2414,7 +2416,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>28575</xdr:colOff>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>13</xdr:row>
                     <xdr:rowOff>19050</xdr:rowOff>
                   </to>
@@ -2436,7 +2438,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>28575</xdr:colOff>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>17</xdr:row>
                     <xdr:rowOff>19050</xdr:rowOff>
                   </to>
@@ -2458,7 +2460,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>28575</xdr:colOff>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>18</xdr:row>
                     <xdr:rowOff>19050</xdr:rowOff>
                   </to>
@@ -2480,7 +2482,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>28575</xdr:colOff>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>19</xdr:row>
                     <xdr:rowOff>19050</xdr:rowOff>
                   </to>
@@ -2497,13 +2499,35 @@
                   <from>
                     <xdr:col>3</xdr:col>
                     <xdr:colOff>76200</xdr:colOff>
+                    <xdr:row>19</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>20</xdr:row>
+                    <xdr:rowOff>28575</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="2060" r:id="rId12" name="Check Box 12">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>76200</xdr:colOff>
+                    <xdr:row>25</xdr:row>
                     <xdr:rowOff>180975</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>28575</xdr:colOff>
-                    <xdr:row>22</xdr:row>
+                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:row>27</xdr:row>
                     <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
@@ -2513,19 +2537,19 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="2058" r:id="rId12" name="Check Box 10">
+            <control shapeId="2061" r:id="rId13" name="Check Box 13">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>3</xdr:col>
                     <xdr:colOff>76200</xdr:colOff>
-                    <xdr:row>22</xdr:row>
+                    <xdr:row>28</xdr:row>
                     <xdr:rowOff>180975</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>28575</xdr:colOff>
-                    <xdr:row>24</xdr:row>
+                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:row>30</xdr:row>
                     <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
@@ -2535,29 +2559,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="2060" r:id="rId13" name="Check Box 12">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>3</xdr:col>
-                    <xdr:colOff>76200</xdr:colOff>
-                    <xdr:row>26</xdr:row>
-                    <xdr:rowOff>180975</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>4</xdr:col>
-                    <xdr:colOff>28575</xdr:colOff>
-                    <xdr:row>28</xdr:row>
-                    <xdr:rowOff>19050</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="2061" r:id="rId14" name="Check Box 13">
+            <control shapeId="2062" r:id="rId14" name="Check Box 14">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -2568,7 +2570,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>28575</xdr:colOff>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>31</xdr:row>
                     <xdr:rowOff>19050</xdr:rowOff>
                   </to>
@@ -2579,7 +2581,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="2062" r:id="rId15" name="Check Box 14">
+            <control shapeId="2063" r:id="rId15" name="Check Box 15">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -2590,7 +2592,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>28575</xdr:colOff>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>32</xdr:row>
                     <xdr:rowOff>19050</xdr:rowOff>
                   </to>
@@ -2601,7 +2603,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="2063" r:id="rId16" name="Check Box 15">
+            <control shapeId="2064" r:id="rId16" name="Check Box 16">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -2612,7 +2614,7 @@
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>28575</xdr:colOff>
+                    <xdr:colOff>104775</xdr:colOff>
                     <xdr:row>33</xdr:row>
                     <xdr:rowOff>19050</xdr:rowOff>
                   </to>
@@ -2623,19 +2625,19 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="2064" r:id="rId17" name="Check Box 16">
+            <control shapeId="2067" r:id="rId17" name="Check Box 19">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>3</xdr:col>
                     <xdr:colOff>76200</xdr:colOff>
-                    <xdr:row>32</xdr:row>
+                    <xdr:row>35</xdr:row>
                     <xdr:rowOff>180975</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>28575</xdr:colOff>
-                    <xdr:row>34</xdr:row>
+                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:row>37</xdr:row>
                     <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
@@ -2645,19 +2647,41 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="2067" r:id="rId18" name="Check Box 19">
+            <control shapeId="2068" r:id="rId18" name="Check Box 20">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>3</xdr:col>
                     <xdr:colOff>76200</xdr:colOff>
-                    <xdr:row>36</xdr:row>
+                    <xdr:row>19</xdr:row>
+                    <xdr:rowOff>171450</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:row>21</xdr:row>
+                    <xdr:rowOff>9525</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="2069" r:id="rId19" name="Check Box 21">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>76200</xdr:colOff>
+                    <xdr:row>21</xdr:row>
                     <xdr:rowOff>180975</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>28575</xdr:colOff>
-                    <xdr:row>38</xdr:row>
+                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:row>23</xdr:row>
                     <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>

</xml_diff>